<commit_message>
Added level shifter info
</commit_message>
<xml_diff>
--- a/_applications2/902_drivers/assets/types.xlsx
+++ b/_applications2/902_drivers/assets/types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lutz\source\WebSites\ghPages-TeensyStep\_applications2\902_drivers\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B04615-8294-4791-A382-3A534E451FA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BED446-83A6-4441-84B4-E5C8381CAA1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFA014E0-0A27-413C-A3F6-05D46AB5599E}"/>
   </bookViews>
@@ -69,13 +69,7 @@
     <t>up to 1/256</t>
   </si>
   <si>
-    <t>Classic driver for 3d printers</t>
-  </si>
-  <si>
     <t>Driver</t>
-  </si>
-  <si>
-    <t>More robust than A4988</t>
   </si>
   <si>
     <r>
@@ -441,13 +435,6 @@
   </si>
   <si>
     <t>20-50V</t>
-  </si>
-  <si>
-    <t>Aka ‘SilentStepStick’
-STP/DIR and SPI interface</t>
-  </si>
-  <si>
-    <t>Low current version of DRV8825</t>
   </si>
   <si>
     <t>Automatic current reduction 
@@ -462,6 +449,18 @@
 200kHz max, 
 Very smooth movement
 Self-test and auto-setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic driver for 3d printers. A lot of breakout boards are available. </t>
+  </si>
+  <si>
+    <t>More robust than A4988.</t>
+  </si>
+  <si>
+    <t>Low current version of DRV8825. Easier to adjust the motor current for small motors.</t>
+  </si>
+  <si>
+    <t>Aka ‘SilentStepStick’. Can be controlled via a STP / DIR / mode pins and / or a SPI interface</t>
   </si>
 </sst>
 </file>
@@ -554,16 +553,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -572,28 +601,43 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -602,43 +646,43 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -647,79 +691,40 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="hair">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -731,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -745,64 +750,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1122,7 +1136,7 @@
   <dimension ref="B1:G8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,149 +1147,149 @@
     <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" s="4" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>23</v>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>12</v>
+      <c r="G3" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>14</v>
+      <c r="G7" s="19" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    <row r="8" spans="2:7" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="23" t="s">
+      <c r="F8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="27" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>